<commit_message>
added download for file. added water deficit slider.
</commit_message>
<xml_diff>
--- a/data/heliaphen_experiments.xlsx
+++ b/data/heliaphen_experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="heliaphen_experiments" sheetId="1" state="visible" r:id="rId2"/>
@@ -208,18 +208,18 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="127.25"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.89795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.4387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="162.352040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="5.93877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="16.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,7 +306,7 @@
         <v>96</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,7 +335,7 @@
         <v>96</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +364,7 @@
         <v>96</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,7 +393,7 @@
         <v>192</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,7 +416,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added visualization for water extraction and slider for soil water capacity parameter
</commit_message>
<xml_diff>
--- a/data/heliaphen_experiments.xlsx
+++ b/data/heliaphen_experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="heliaphen_experiments" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t xml:space="preserve">experiment</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t xml:space="preserve">15HP04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-06-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-06-12</t>
   </si>
   <si>
     <t xml:space="preserve">15HP05</t>
@@ -114,7 +120,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,16 +142,139 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -153,8 +282,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,6 +322,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -189,14 +381,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -207,19 +475,19 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85"/>
+  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="183.408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.7602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="6.65816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="18.3571428571429"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="112.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="6.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="18.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>16</v>
@@ -398,10 +666,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -421,10 +689,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -445,7 +713,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
added export for water deficit table
</commit_message>
<xml_diff>
--- a/data/heliaphen_experiments.xlsx
+++ b/data/heliaphen_experiments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">experiment</t>
   </si>
@@ -55,24 +55,12 @@
     <t xml:space="preserve">déterminer la sensibilité au déficit hydrique pour des hybrides commerciaux récents</t>
   </si>
   <si>
-    <t xml:space="preserve">2014-06-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014-06-17</t>
-  </si>
-  <si>
     <t xml:space="preserve">15HP01</t>
   </si>
   <si>
     <t xml:space="preserve">analyser l'effet d'une différence de demande évaporative sur la sensibilité au déficit hydrique (semis 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">2015-05-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-05-21</t>
-  </si>
-  <si>
     <t xml:space="preserve">15HP02</t>
   </si>
   <si>
@@ -85,21 +73,9 @@
     <t xml:space="preserve">analyser l'effet d'une différence de demande évaporative sur la sensibilité au déficit hydrique (semis 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">2015-09-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-10-19</t>
-  </si>
-  <si>
     <t xml:space="preserve">15HP04</t>
   </si>
   <si>
-    <t xml:space="preserve">2015-06-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-06-12</t>
-  </si>
-  <si>
     <t xml:space="preserve">15HP05</t>
   </si>
   <si>
@@ -110,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">analyser le lien entre sensibilite au déficit hydrique identifié au champ (regressions) ou sur la plateforme (biomasse produite) en stress fixe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16HP08</t>
   </si>
 </sst>
 </file>
@@ -118,9 +97,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,6 +198,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -371,13 +357,25 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -473,64 +471,64 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="112.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="112.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="14.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="6.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="18.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
+      <c r="C2" s="4" t="n">
+        <v>41794</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>41807</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>16</v>
@@ -548,18 +546,18 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>42128</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>42145</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>8</v>
@@ -577,18 +575,18 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>42128</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>42145</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8</v>
@@ -606,18 +604,18 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>42277</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>42296</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>8</v>
@@ -635,18 +633,18 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
+      <c r="C6" s="4" t="n">
+        <v>42158</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>42167</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>16</v>
@@ -664,18 +662,18 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>42128</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>42145</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>24</v>
@@ -687,18 +685,18 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>42128</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>42145</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>24</v>
@@ -708,6 +706,35 @@
       </c>
       <c r="I8" s="0" t="n">
         <v>1300</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>42511</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>42524</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected tooltip format for ggplotly graphics
</commit_message>
<xml_diff>
--- a/data/heliaphen_experiments.xlsx
+++ b/data/heliaphen_experiments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">experiment</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">weight_dead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13HP02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biologie des systèmes</t>
   </si>
   <si>
     <t xml:space="preserve">14HP09</t>
@@ -99,7 +105,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -123,94 +129,13 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,48 +144,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -268,23 +157,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,54 +182,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -366,11 +192,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,44 +205,28 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -444,7 +254,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -471,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -525,22 +335,16 @@
         <v>10</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>41794</v>
+        <v>41463</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>41807</v>
+        <v>41467</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>192</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>450</v>
@@ -554,13 +358,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>42128</v>
+        <v>41794</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>42145</v>
+        <v>41807</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
@@ -569,10 +373,10 @@
         <v>6</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>1300</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,10 +416,10 @@
         <v>16</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>42277</v>
+        <v>42128</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>42296</v>
+        <v>42145</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>8</v>
@@ -638,16 +442,16 @@
         <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>42158</v>
+        <v>42277</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>42167</v>
+        <v>42296</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
@@ -656,7 +460,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>1300</v>
@@ -664,22 +468,28 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>42128</v>
+        <v>42158</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>42145</v>
+        <v>42167</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1300</v>
@@ -713,27 +523,50 @@
         <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>42128</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>42145</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>42511</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>42524</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>42511</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>42524</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H9" s="0" t="n">
+      <c r="F10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>1127</v>
       </c>
     </row>

</xml_diff>